<commit_message>
18.05.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Requisition/May/17.05.2020 Requisition of Mugdho Corporation.xlsx
+++ b/2020/Requisition/May/17.05.2020 Requisition of Mugdho Corporation.xlsx
@@ -1097,13 +1097,13 @@
       <pane xSplit="4" ySplit="14" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="I104" sqref="I104"/>
+      <selection pane="bottomRight" activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="25.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="30" style="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>

</xml_diff>